<commit_message>
update plan result 20200910 at 13:00
</commit_message>
<xml_diff>
--- a/20200910.xlsx
+++ b/20200910.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swan3\Desktop\계획\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swan3\Desktop\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB84A8AE-39F8-487C-B7D6-15BD20A6722C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39AF7B6-BD8A-4909-8896-CF5F7D2547C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24000" yWindow="264" windowWidth="21600" windowHeight="11388" tabRatio="580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24276" yWindow="540" windowWidth="21600" windowHeight="11388" tabRatio="580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
   <si>
     <t>내용</t>
   </si>
@@ -204,6 +204,11 @@
   </si>
   <si>
     <t>소켓 코딩</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>핸드폰 꺼져서 지각
+10:00부터 진행했음</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
 </sst>
@@ -367,7 +372,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -566,8 +571,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -758,6 +775,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -893,7 +947,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -957,14 +1011,41 @@
     <xf numFmtId="0" fontId="0" fillId="32" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -978,32 +1059,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1532,7 +1604,7 @@
   <dimension ref="B2:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C8"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1581,13 +1653,13 @@
       <c r="B3" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="31"/>
+      <c r="E3" s="37"/>
       <c r="F3" s="17"/>
       <c r="H3" t="s">
         <v>28</v>
@@ -1600,10 +1672,10 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="23"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="31"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="37"/>
       <c r="F4" s="17"/>
       <c r="H4" t="s">
         <v>30</v>
@@ -1613,10 +1685,10 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="31"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="37"/>
       <c r="F5" s="17"/>
       <c r="H5" t="s">
         <v>29</v>
@@ -1626,10 +1698,10 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="23"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="31"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="37"/>
       <c r="F6" s="17"/>
       <c r="H6" t="s">
         <v>25</v>
@@ -1639,10 +1711,10 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="31"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="37"/>
       <c r="F7" s="17"/>
       <c r="H7" t="s">
         <v>19</v>
@@ -1656,10 +1728,10 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="23"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="31"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="37"/>
       <c r="F8" s="17"/>
       <c r="H8" t="s">
         <v>22</v>
@@ -1675,9 +1747,11 @@
       <c r="C9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="17"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="42" t="s">
+        <v>55</v>
+      </c>
       <c r="H9" t="s">
         <v>23</v>
       </c>
@@ -1695,22 +1769,22 @@
       <c r="C10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="17"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="40"/>
     </row>
     <row r="11" spans="2:12" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="31"/>
-      <c r="F11" s="17"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="41"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
@@ -1719,19 +1793,19 @@
       <c r="C12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="31"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="17"/>
     </row>
     <row r="13" spans="2:12" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="31"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="18"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
@@ -1741,8 +1815,8 @@
       <c r="C14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="31"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="18"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
@@ -1752,8 +1826,8 @@
       <c r="C15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="31"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="21"/>
       <c r="F15" s="18"/>
     </row>
     <row r="16" spans="2:12" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1763,9 +1837,9 @@
       <c r="C16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="21"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="28"/>
     </row>
     <row r="17" spans="2:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
@@ -1774,9 +1848,9 @@
       <c r="C17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="21"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="28"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
@@ -1785,8 +1859,8 @@
       <c r="C18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="27"/>
-      <c r="E18" s="31"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="21"/>
       <c r="F18" s="18"/>
     </row>
     <row r="19" spans="2:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1796,10 +1870,10 @@
       <c r="C19" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="32"/>
+      <c r="E19" s="22"/>
       <c r="F19" s="18"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
@@ -1809,8 +1883,8 @@
       <c r="C20" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="28"/>
-      <c r="E20" s="33"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="23"/>
       <c r="F20" s="18"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
@@ -1820,8 +1894,8 @@
       <c r="C21" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="28"/>
-      <c r="E21" s="34"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="24"/>
       <c r="F21" s="18"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
@@ -1831,8 +1905,8 @@
       <c r="C22" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="28"/>
-      <c r="E22" s="34"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="24"/>
       <c r="F22" s="19"/>
     </row>
     <row r="23" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1842,8 +1916,8 @@
       <c r="C23" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="28"/>
-      <c r="E23" s="34"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="24"/>
       <c r="F23" s="20"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
@@ -1855,13 +1929,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="D19:D23"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="C3:C8"/>
     <mergeCell ref="D3:D10"/>
     <mergeCell ref="D11:D18"/>
+    <mergeCell ref="F9:F11"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.69972223043441772" right="0.69972223043441772" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>

</xml_diff>